<commit_message>
update TAL ferm improvements scenario and minor plotting changes
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_B.xlsx
+++ b/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_B.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\biorefineries\TAL\analyses\full\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A11373-2926-4938-B465-9F0E1F6B16B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E3233F-586A-4896-8F8D-68B4BE117B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -835,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1593,19 +1593,19 @@
         <v>20</v>
       </c>
       <c r="E23" s="7">
-        <v>0.68</v>
+        <v>0.73</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G23" s="7">
         <f>0.8*E23</f>
-        <v>0.54400000000000004</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="7">
         <f>1.2*E23</f>
-        <v>0.81600000000000006</v>
+        <v>0.876</v>
       </c>
       <c r="J23" s="7"/>
       <c r="K23" s="7" t="s">
@@ -1626,19 +1626,19 @@
         <v>12</v>
       </c>
       <c r="E24" s="7">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G24" s="7">
         <f>E24*0.8</f>
-        <v>60.800000000000004</v>
+        <v>54.400000000000006</v>
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="7">
         <f>E24*1.2</f>
-        <v>91.2</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="J24" s="7"/>
       <c r="K24" s="7" t="s">

</xml_diff>